<commit_message>
add new asset v1
</commit_message>
<xml_diff>
--- a/Docs/Assets_Template_ updated final.xlsx
+++ b/Docs/Assets_Template_ updated final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\logistic\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEA2336-C3AC-4940-9CE5-193AEE33826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47942D81-A221-4F8F-9BF1-B5B0E21DFAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="769" activeTab="1" xr2:uid="{CB6DDDD5-16B0-448E-8171-F32A2B4AEEC5}"/>
+    <workbookView xWindow="-23136" yWindow="-24" windowWidth="23232" windowHeight="12432" tabRatio="769" activeTab="6" xr2:uid="{CB6DDDD5-16B0-448E-8171-F32A2B4AEEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="suppliers" sheetId="7" r:id="rId1"/>
@@ -5306,8 +5306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86060676-D353-469D-B400-DC39E59A0722}">
   <dimension ref="A1:S180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10592,8 +10592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D011BDFC-04A7-4A03-9396-91A8DE874C29}">
   <dimension ref="A1:W4549"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -48308,7 +48308,7 @@
   <dimension ref="A1:AA155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -49364,8 +49364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AAF5DE-78EF-42C9-9FE8-41208EDCE960}">
   <dimension ref="A1:AF298"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" activeCellId="1" sqref="A1:AF298"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
data import from excel
</commit_message>
<xml_diff>
--- a/Docs/Assets_Template_ updated final.xlsx
+++ b/Docs/Assets_Template_ updated final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\logistic\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C88DCE-4CF1-4846-80FE-0F31A23DAF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59607F5-8F57-48E0-ADB7-4100C04AE11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="769" activeTab="3" xr2:uid="{CB6DDDD5-16B0-448E-8171-F32A2B4AEEC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="769" activeTab="6" xr2:uid="{CB6DDDD5-16B0-448E-8171-F32A2B4AEEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="suppliers" sheetId="7" r:id="rId1"/>
@@ -3301,10 +3301,28 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3315,24 +3333,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5308,8 +5308,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S180"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5365,7 +5365,7 @@
       <c r="A2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="104" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4"/>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="98"/>
-      <c r="B3" s="97"/>
+      <c r="B3" s="104"/>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
@@ -5412,7 +5412,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="98"/>
-      <c r="B4" s="97"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
@@ -5443,7 +5443,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="98"/>
-      <c r="B5" s="97"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="98"/>
-      <c r="B6" s="97"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="98"/>
-      <c r="B7" s="97"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="98"/>
-      <c r="B8" s="97"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -5553,7 +5553,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="98"/>
-      <c r="B9" s="97"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
@@ -5574,7 +5574,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="98"/>
-      <c r="B10" s="97"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
@@ -5589,7 +5589,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="98"/>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="105" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5"/>
@@ -5608,7 +5608,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="98"/>
-      <c r="B12" s="99"/>
+      <c r="B12" s="105"/>
       <c r="C12" s="5" t="s">
         <v>60</v>
       </c>
@@ -5627,7 +5627,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="98"/>
-      <c r="B13" s="99"/>
+      <c r="B13" s="105"/>
       <c r="C13" s="5" t="s">
         <v>61</v>
       </c>
@@ -5646,7 +5646,7 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="98"/>
-      <c r="B14" s="99"/>
+      <c r="B14" s="105"/>
       <c r="C14" s="5" t="s">
         <v>62</v>
       </c>
@@ -5665,7 +5665,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="98"/>
-      <c r="B15" s="99"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="5" t="s">
         <v>63</v>
       </c>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="98"/>
-      <c r="B16" s="99"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
         <v>67</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="98"/>
-      <c r="B17" s="99"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
         <v>68</v>
@@ -5718,7 +5718,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="98"/>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="104" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="4"/>
@@ -5737,7 +5737,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="98"/>
-      <c r="B19" s="97"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="4" t="s">
         <v>7</v>
       </c>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="98"/>
-      <c r="B20" s="97"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="4" t="s">
         <v>74</v>
       </c>
@@ -5775,7 +5775,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="98"/>
-      <c r="B21" s="97"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="4" t="s">
         <v>75</v>
       </c>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="22" spans="1:17" ht="15">
       <c r="A22" s="98"/>
-      <c r="B22" s="97"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="4" t="s">
         <v>76</v>
       </c>
@@ -5812,7 +5812,7 @@
     </row>
     <row r="23" spans="1:17" ht="15">
       <c r="A23" s="98"/>
-      <c r="B23" s="97"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
         <v>67</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="24" spans="1:17" ht="15">
       <c r="A24" s="98"/>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="105" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="6"/>
@@ -5844,7 +5844,7 @@
     </row>
     <row r="25" spans="1:17" ht="15.75">
       <c r="A25" s="98"/>
-      <c r="B25" s="99"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="6" t="s">
         <v>81</v>
       </c>
@@ -5860,7 +5860,7 @@
     </row>
     <row r="26" spans="1:17" ht="15">
       <c r="A26" s="98"/>
-      <c r="B26" s="99"/>
+      <c r="B26" s="105"/>
       <c r="C26" s="6" t="s">
         <v>82</v>
       </c>
@@ -5877,7 +5877,7 @@
     </row>
     <row r="27" spans="1:17" ht="15">
       <c r="A27" s="98"/>
-      <c r="B27" s="99"/>
+      <c r="B27" s="105"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6" t="s">
         <v>84</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="28" spans="1:17" ht="15">
       <c r="A28" s="98"/>
-      <c r="B28" s="99"/>
+      <c r="B28" s="105"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6" t="s">
         <v>78</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="98"/>
-      <c r="B29" s="100" t="s">
+      <c r="B29" s="106" t="s">
         <v>85</v>
       </c>
       <c r="C29" s="4"/>
@@ -5920,7 +5920,7 @@
     </row>
     <row r="30" spans="1:17" ht="15.75">
       <c r="A30" s="98"/>
-      <c r="B30" s="100"/>
+      <c r="B30" s="106"/>
       <c r="C30" s="4" t="s">
         <v>86</v>
       </c>
@@ -5937,7 +5937,7 @@
     </row>
     <row r="31" spans="1:17" ht="15.75">
       <c r="A31" s="98"/>
-      <c r="B31" s="100"/>
+      <c r="B31" s="106"/>
       <c r="C31" s="4" t="s">
         <v>87</v>
       </c>
@@ -5954,7 +5954,7 @@
     </row>
     <row r="32" spans="1:17" ht="15">
       <c r="A32" s="98"/>
-      <c r="B32" s="100"/>
+      <c r="B32" s="106"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="7" t="s">
@@ -5966,7 +5966,7 @@
     </row>
     <row r="33" spans="1:16" ht="15">
       <c r="A33" s="98"/>
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="107" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="6"/>
@@ -5983,7 +5983,7 @@
     </row>
     <row r="34" spans="1:16" ht="15" customHeight="1">
       <c r="A34" s="98"/>
-      <c r="B34" s="101"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="6" t="s">
         <v>94</v>
       </c>
@@ -6000,7 +6000,7 @@
     </row>
     <row r="35" spans="1:16" ht="15">
       <c r="A35" s="98"/>
-      <c r="B35" s="101"/>
+      <c r="B35" s="107"/>
       <c r="C35" s="6" t="s">
         <v>95</v>
       </c>
@@ -6017,7 +6017,7 @@
     </row>
     <row r="36" spans="1:16" ht="15">
       <c r="A36" s="98"/>
-      <c r="B36" s="102" t="s">
+      <c r="B36" s="100" t="s">
         <v>211</v>
       </c>
       <c r="C36" s="7"/>
@@ -6034,7 +6034,7 @@
     </row>
     <row r="37" spans="1:16" ht="15">
       <c r="A37" s="98"/>
-      <c r="B37" s="102"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="7" t="s">
         <v>97</v>
       </c>
@@ -6051,7 +6051,7 @@
     </row>
     <row r="38" spans="1:16" ht="15">
       <c r="A38" s="98"/>
-      <c r="B38" s="102"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7" t="s">
         <v>64</v>
@@ -6066,7 +6066,7 @@
     </row>
     <row r="39" spans="1:16" ht="15">
       <c r="A39" s="98"/>
-      <c r="B39" s="102"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
@@ -6079,7 +6079,7 @@
     </row>
     <row r="40" spans="1:16" ht="15">
       <c r="A40" s="98"/>
-      <c r="B40" s="103" t="s">
+      <c r="B40" s="102" t="s">
         <v>212</v>
       </c>
       <c r="C40" s="6"/>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="41" spans="1:16" ht="15">
       <c r="A41" s="98"/>
-      <c r="B41" s="103"/>
+      <c r="B41" s="102"/>
       <c r="C41" s="6" t="s">
         <v>214</v>
       </c>
@@ -6112,7 +6112,7 @@
     </row>
     <row r="42" spans="1:16" ht="15">
       <c r="A42" s="98"/>
-      <c r="B42" s="103"/>
+      <c r="B42" s="102"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
         <v>66</v>
@@ -6127,7 +6127,7 @@
     </row>
     <row r="43" spans="1:16" ht="15">
       <c r="A43" s="98"/>
-      <c r="B43" s="103"/>
+      <c r="B43" s="102"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6" t="s">
@@ -6140,7 +6140,7 @@
     </row>
     <row r="44" spans="1:16" ht="15">
       <c r="A44" s="98"/>
-      <c r="B44" s="102" t="s">
+      <c r="B44" s="100" t="s">
         <v>213</v>
       </c>
       <c r="C44" s="7"/>
@@ -6157,7 +6157,7 @@
     </row>
     <row r="45" spans="1:16" ht="15">
       <c r="A45" s="98"/>
-      <c r="B45" s="102"/>
+      <c r="B45" s="100"/>
       <c r="C45" s="7" t="s">
         <v>101</v>
       </c>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="46" spans="1:16" ht="15">
       <c r="A46" s="98"/>
-      <c r="B46" s="102"/>
+      <c r="B46" s="100"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -6191,7 +6191,7 @@
     </row>
     <row r="47" spans="1:16" ht="15">
       <c r="A47" s="98"/>
-      <c r="B47" s="102"/>
+      <c r="B47" s="100"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
@@ -6209,10 +6209,10 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="15">
-      <c r="A49" s="105" t="s">
+      <c r="A49" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="102" t="s">
+      <c r="B49" s="100" t="s">
         <v>104</v>
       </c>
       <c r="C49" s="7"/>
@@ -6228,8 +6228,8 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="15">
-      <c r="A50" s="105"/>
-      <c r="B50" s="102"/>
+      <c r="A50" s="103"/>
+      <c r="B50" s="100"/>
       <c r="C50" s="7" t="s">
         <v>105</v>
       </c>
@@ -6245,8 +6245,8 @@
       </c>
     </row>
     <row r="51" spans="1:16" ht="15">
-      <c r="A51" s="105"/>
-      <c r="B51" s="102"/>
+      <c r="A51" s="103"/>
+      <c r="B51" s="100"/>
       <c r="C51" s="7" t="s">
         <v>107</v>
       </c>
@@ -6262,8 +6262,8 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15">
-      <c r="A52" s="105"/>
-      <c r="B52" s="102"/>
+      <c r="A52" s="103"/>
+      <c r="B52" s="100"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7" t="s">
         <v>109</v>
@@ -6277,8 +6277,8 @@
       </c>
     </row>
     <row r="53" spans="1:16" ht="15">
-      <c r="A53" s="105"/>
-      <c r="B53" s="102"/>
+      <c r="A53" s="103"/>
+      <c r="B53" s="100"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7">
@@ -6290,7 +6290,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" ht="15">
-      <c r="A54" s="105"/>
+      <c r="A54" s="103"/>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
         <v>215</v>
@@ -6307,8 +6307,8 @@
       </c>
     </row>
     <row r="55" spans="1:16" ht="15">
-      <c r="A55" s="105"/>
-      <c r="B55" s="104" t="s">
+      <c r="A55" s="103"/>
+      <c r="B55" s="99" t="s">
         <v>110</v>
       </c>
       <c r="C55" s="6" t="s">
@@ -6326,8 +6326,8 @@
       </c>
     </row>
     <row r="56" spans="1:16" ht="15">
-      <c r="A56" s="105"/>
-      <c r="B56" s="104"/>
+      <c r="A56" s="103"/>
+      <c r="B56" s="99"/>
       <c r="C56" s="6" t="s">
         <v>112</v>
       </c>
@@ -6343,8 +6343,8 @@
       </c>
     </row>
     <row r="57" spans="1:16" ht="15">
-      <c r="A57" s="105"/>
-      <c r="B57" s="104"/>
+      <c r="A57" s="103"/>
+      <c r="B57" s="99"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6" t="s">
@@ -6356,8 +6356,8 @@
       </c>
     </row>
     <row r="58" spans="1:16" ht="15">
-      <c r="A58" s="105"/>
-      <c r="B58" s="104"/>
+      <c r="A58" s="103"/>
+      <c r="B58" s="99"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6" t="s">
@@ -6369,7 +6369,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" ht="15">
-      <c r="A59" s="105"/>
+      <c r="A59" s="103"/>
       <c r="B59" s="57"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -6382,8 +6382,8 @@
       </c>
     </row>
     <row r="60" spans="1:16" ht="15">
-      <c r="A60" s="105"/>
-      <c r="B60" s="102" t="s">
+      <c r="A60" s="103"/>
+      <c r="B60" s="100" t="s">
         <v>116</v>
       </c>
       <c r="C60" s="7" t="s">
@@ -6401,8 +6401,8 @@
       </c>
     </row>
     <row r="61" spans="1:16" ht="15">
-      <c r="A61" s="105"/>
-      <c r="B61" s="102"/>
+      <c r="A61" s="103"/>
+      <c r="B61" s="100"/>
       <c r="C61" s="7" t="s">
         <v>116</v>
       </c>
@@ -6418,8 +6418,8 @@
       </c>
     </row>
     <row r="62" spans="1:16" ht="16.899999999999999" customHeight="1">
-      <c r="A62" s="105"/>
-      <c r="B62" s="102"/>
+      <c r="A62" s="103"/>
+      <c r="B62" s="100"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
@@ -6431,7 +6431,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" ht="16.899999999999999" customHeight="1">
-      <c r="A63" s="105"/>
+      <c r="A63" s="103"/>
       <c r="B63" s="8"/>
       <c r="C63" s="61"/>
       <c r="D63" s="6"/>
@@ -6444,8 +6444,8 @@
       </c>
     </row>
     <row r="64" spans="1:16" ht="15">
-      <c r="A64" s="105"/>
-      <c r="B64" s="104" t="s">
+      <c r="A64" s="103"/>
+      <c r="B64" s="99" t="s">
         <v>121</v>
       </c>
       <c r="C64" s="6"/>
@@ -6461,8 +6461,8 @@
       </c>
     </row>
     <row r="65" spans="1:16" ht="15">
-      <c r="A65" s="105"/>
-      <c r="B65" s="104"/>
+      <c r="A65" s="103"/>
+      <c r="B65" s="99"/>
       <c r="C65" s="6" t="s">
         <v>121</v>
       </c>
@@ -6478,8 +6478,8 @@
       </c>
     </row>
     <row r="66" spans="1:16" ht="15">
-      <c r="A66" s="105"/>
-      <c r="B66" s="104"/>
+      <c r="A66" s="103"/>
+      <c r="B66" s="99"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6" t="s">
@@ -6491,7 +6491,7 @@
       </c>
     </row>
     <row r="67" spans="1:16" ht="15">
-      <c r="A67" s="105"/>
+      <c r="A67" s="103"/>
       <c r="B67" s="10" t="s">
         <v>242</v>
       </c>
@@ -6510,8 +6510,8 @@
       </c>
     </row>
     <row r="68" spans="1:16" ht="15">
-      <c r="A68" s="105"/>
-      <c r="B68" s="104" t="s">
+      <c r="A68" s="103"/>
+      <c r="B68" s="99" t="s">
         <v>243</v>
       </c>
       <c r="C68" s="6"/>
@@ -6527,8 +6527,8 @@
       </c>
     </row>
     <row r="69" spans="1:16" ht="15">
-      <c r="A69" s="105"/>
-      <c r="B69" s="104"/>
+      <c r="A69" s="103"/>
+      <c r="B69" s="99"/>
       <c r="C69" s="6" t="s">
         <v>126</v>
       </c>
@@ -6544,8 +6544,8 @@
       </c>
     </row>
     <row r="70" spans="1:16" ht="15">
-      <c r="A70" s="105"/>
-      <c r="B70" s="104"/>
+      <c r="A70" s="103"/>
+      <c r="B70" s="99"/>
       <c r="C70" s="6" t="s">
         <v>128</v>
       </c>
@@ -6559,8 +6559,8 @@
       </c>
     </row>
     <row r="71" spans="1:16" ht="15">
-      <c r="A71" s="105"/>
-      <c r="B71" s="104"/>
+      <c r="A71" s="103"/>
+      <c r="B71" s="99"/>
       <c r="C71" s="6" t="s">
         <v>130</v>
       </c>
@@ -6574,8 +6574,8 @@
       </c>
     </row>
     <row r="72" spans="1:16" ht="15">
-      <c r="A72" s="105"/>
-      <c r="B72" s="104"/>
+      <c r="A72" s="103"/>
+      <c r="B72" s="99"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6" t="s">
@@ -6587,8 +6587,8 @@
       </c>
     </row>
     <row r="73" spans="1:16" ht="15">
-      <c r="A73" s="105"/>
-      <c r="B73" s="104"/>
+      <c r="A73" s="103"/>
+      <c r="B73" s="99"/>
       <c r="C73" s="61"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6" t="s">
@@ -6600,8 +6600,8 @@
       </c>
     </row>
     <row r="74" spans="1:16" ht="15">
-      <c r="A74" s="105"/>
-      <c r="B74" s="102" t="s">
+      <c r="A74" s="103"/>
+      <c r="B74" s="100" t="s">
         <v>134</v>
       </c>
       <c r="C74" s="7"/>
@@ -6617,8 +6617,8 @@
       </c>
     </row>
     <row r="75" spans="1:16" ht="15">
-      <c r="A75" s="105"/>
-      <c r="B75" s="102"/>
+      <c r="A75" s="103"/>
+      <c r="B75" s="100"/>
       <c r="C75" s="7" t="s">
         <v>135</v>
       </c>
@@ -6634,8 +6634,8 @@
       </c>
     </row>
     <row r="76" spans="1:16" ht="15">
-      <c r="A76" s="105"/>
-      <c r="B76" s="102"/>
+      <c r="A76" s="103"/>
+      <c r="B76" s="100"/>
       <c r="C76" s="7" t="s">
         <v>136</v>
       </c>
@@ -6649,8 +6649,8 @@
       </c>
     </row>
     <row r="77" spans="1:16" ht="15">
-      <c r="A77" s="105"/>
-      <c r="B77" s="102"/>
+      <c r="A77" s="103"/>
+      <c r="B77" s="100"/>
       <c r="C77" s="7" t="s">
         <v>137</v>
       </c>
@@ -6661,8 +6661,8 @@
       </c>
     </row>
     <row r="78" spans="1:16" ht="15">
-      <c r="A78" s="105"/>
-      <c r="B78" s="102"/>
+      <c r="A78" s="103"/>
+      <c r="B78" s="100"/>
       <c r="C78" s="7" t="s">
         <v>138</v>
       </c>
@@ -6673,8 +6673,8 @@
       </c>
     </row>
     <row r="79" spans="1:16" ht="15">
-      <c r="A79" s="105"/>
-      <c r="B79" s="102"/>
+      <c r="A79" s="103"/>
+      <c r="B79" s="100"/>
       <c r="C79" s="7" t="s">
         <v>139</v>
       </c>
@@ -6685,8 +6685,8 @@
       </c>
     </row>
     <row r="80" spans="1:16" ht="15">
-      <c r="A80" s="105"/>
-      <c r="B80" s="102"/>
+      <c r="A80" s="103"/>
+      <c r="B80" s="100"/>
       <c r="C80" s="7" t="s">
         <v>140</v>
       </c>
@@ -6694,7 +6694,7 @@
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:14" ht="15">
-      <c r="A81" s="105"/>
+      <c r="A81" s="103"/>
       <c r="B81" s="8"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7" t="s">
@@ -6705,8 +6705,8 @@
       </c>
     </row>
     <row r="82" spans="1:14" ht="15">
-      <c r="A82" s="105"/>
-      <c r="B82" s="104" t="s">
+      <c r="A82" s="103"/>
+      <c r="B82" s="99" t="s">
         <v>141</v>
       </c>
       <c r="C82" s="6" t="s">
@@ -6720,8 +6720,8 @@
       </c>
     </row>
     <row r="83" spans="1:14" ht="15">
-      <c r="A83" s="105"/>
-      <c r="B83" s="104"/>
+      <c r="A83" s="103"/>
+      <c r="B83" s="99"/>
       <c r="C83" s="6" t="s">
         <v>144</v>
       </c>
@@ -6731,8 +6731,8 @@
       </c>
     </row>
     <row r="84" spans="1:14" ht="15">
-      <c r="A84" s="105"/>
-      <c r="B84" s="104"/>
+      <c r="A84" s="103"/>
+      <c r="B84" s="99"/>
       <c r="C84" s="6" t="s">
         <v>146</v>
       </c>
@@ -6742,8 +6742,8 @@
       </c>
     </row>
     <row r="85" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A85" s="105"/>
-      <c r="B85" s="104"/>
+      <c r="A85" s="103"/>
+      <c r="B85" s="99"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6" t="s">
@@ -6751,8 +6751,8 @@
       </c>
     </row>
     <row r="86" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A86" s="105"/>
-      <c r="B86" s="104"/>
+      <c r="A86" s="103"/>
+      <c r="B86" s="99"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6" t="s">
@@ -6761,8 +6761,8 @@
       <c r="N86" s="23"/>
     </row>
     <row r="87" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A87" s="105"/>
-      <c r="B87" s="102" t="s">
+      <c r="A87" s="103"/>
+      <c r="B87" s="100" t="s">
         <v>150</v>
       </c>
       <c r="C87" s="7"/>
@@ -6775,8 +6775,8 @@
       <c r="N87" s="23"/>
     </row>
     <row r="88" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A88" s="105"/>
-      <c r="B88" s="102"/>
+      <c r="A88" s="103"/>
+      <c r="B88" s="100"/>
       <c r="C88" s="7" t="s">
         <v>151</v>
       </c>
@@ -6789,8 +6789,8 @@
       <c r="N88" s="23"/>
     </row>
     <row r="89" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A89" s="105"/>
-      <c r="B89" s="102"/>
+      <c r="A89" s="103"/>
+      <c r="B89" s="100"/>
       <c r="C89" s="7" t="s">
         <v>153</v>
       </c>
@@ -6801,8 +6801,8 @@
       <c r="N89" s="23"/>
     </row>
     <row r="90" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A90" s="105"/>
-      <c r="B90" s="102"/>
+      <c r="A90" s="103"/>
+      <c r="B90" s="100"/>
       <c r="C90" s="7" t="s">
         <v>155</v>
       </c>
@@ -6813,8 +6813,8 @@
       <c r="N90" s="23"/>
     </row>
     <row r="91" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A91" s="105"/>
-      <c r="B91" s="102"/>
+      <c r="A91" s="103"/>
+      <c r="B91" s="100"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="7" t="s">
@@ -6823,7 +6823,7 @@
       <c r="N91" s="23"/>
     </row>
     <row r="92" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A92" s="105"/>
+      <c r="A92" s="103"/>
       <c r="B92" s="11" t="s">
         <v>158</v>
       </c>
@@ -6839,8 +6839,8 @@
       <c r="N92" s="23"/>
     </row>
     <row r="93" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A93" s="105"/>
-      <c r="B93" s="102" t="s">
+      <c r="A93" s="103"/>
+      <c r="B93" s="100" t="s">
         <v>244</v>
       </c>
       <c r="C93" s="7"/>
@@ -6851,8 +6851,8 @@
       <c r="N93" s="23"/>
     </row>
     <row r="94" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A94" s="105"/>
-      <c r="B94" s="102"/>
+      <c r="A94" s="103"/>
+      <c r="B94" s="100"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7" t="s">
         <v>215</v>
@@ -6863,8 +6863,8 @@
       <c r="N94" s="23"/>
     </row>
     <row r="95" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A95" s="105"/>
-      <c r="B95" s="102"/>
+      <c r="A95" s="103"/>
+      <c r="B95" s="100"/>
       <c r="C95" s="7" t="s">
         <v>244</v>
       </c>
@@ -6875,8 +6875,8 @@
       <c r="N95" s="23"/>
     </row>
     <row r="96" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A96" s="105"/>
-      <c r="B96" s="104" t="s">
+      <c r="A96" s="103"/>
+      <c r="B96" s="99" t="s">
         <v>249</v>
       </c>
       <c r="C96" s="6"/>
@@ -6889,8 +6889,8 @@
       <c r="N96" s="23"/>
     </row>
     <row r="97" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A97" s="105"/>
-      <c r="B97" s="104"/>
+      <c r="A97" s="103"/>
+      <c r="B97" s="99"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6" t="s">
@@ -6899,8 +6899,8 @@
       <c r="N97" s="23"/>
     </row>
     <row r="98" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A98" s="105"/>
-      <c r="B98" s="104"/>
+      <c r="A98" s="103"/>
+      <c r="B98" s="99"/>
       <c r="C98" s="6" t="s">
         <v>249</v>
       </c>
@@ -6911,8 +6911,8 @@
       <c r="N98" s="23"/>
     </row>
     <row r="99" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A99" s="105"/>
-      <c r="B99" s="104"/>
+      <c r="A99" s="103"/>
+      <c r="B99" s="99"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6" t="s">
@@ -6921,7 +6921,7 @@
       <c r="N99" s="24"/>
     </row>
     <row r="100" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A100" s="105"/>
+      <c r="A100" s="103"/>
       <c r="B100" s="57"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
@@ -6931,8 +6931,8 @@
       <c r="N100" s="24"/>
     </row>
     <row r="101" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A101" s="105"/>
-      <c r="B101" s="102" t="s">
+      <c r="A101" s="103"/>
+      <c r="B101" s="100" t="s">
         <v>162</v>
       </c>
       <c r="C101" s="7" t="s">
@@ -6947,8 +6947,8 @@
       <c r="N101" s="24"/>
     </row>
     <row r="102" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A102" s="105"/>
-      <c r="B102" s="102"/>
+      <c r="A102" s="103"/>
+      <c r="B102" s="100"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="7" t="s">
@@ -6957,7 +6957,7 @@
       <c r="N102" s="24"/>
     </row>
     <row r="103" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A103" s="105"/>
+      <c r="A103" s="103"/>
       <c r="B103" s="8"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7" t="s">
@@ -6969,8 +6969,8 @@
       <c r="N103" s="62"/>
     </row>
     <row r="104" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A104" s="105"/>
-      <c r="B104" s="104" t="s">
+      <c r="A104" s="103"/>
+      <c r="B104" s="99" t="s">
         <v>164</v>
       </c>
       <c r="C104" s="6" t="s">
@@ -6983,8 +6983,8 @@
       <c r="N104" s="22"/>
     </row>
     <row r="105" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A105" s="105"/>
-      <c r="B105" s="104"/>
+      <c r="A105" s="103"/>
+      <c r="B105" s="99"/>
       <c r="C105" s="6" t="s">
         <v>164</v>
       </c>
@@ -6995,8 +6995,8 @@
       <c r="N105" s="23"/>
     </row>
     <row r="106" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A106" s="105"/>
-      <c r="B106" s="104"/>
+      <c r="A106" s="103"/>
+      <c r="B106" s="99"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
       <c r="E106" s="6" t="s">
@@ -7005,8 +7005,8 @@
       <c r="N106" s="23"/>
     </row>
     <row r="107" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A107" s="105"/>
-      <c r="B107" s="104"/>
+      <c r="A107" s="103"/>
+      <c r="B107" s="99"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6" t="s">
@@ -7015,8 +7015,8 @@
       <c r="N107" s="23"/>
     </row>
     <row r="108" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A108" s="105"/>
-      <c r="B108" s="104"/>
+      <c r="A108" s="103"/>
+      <c r="B108" s="99"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6" t="s">
@@ -7025,8 +7025,8 @@
       <c r="N108" s="23"/>
     </row>
     <row r="109" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A109" s="105"/>
-      <c r="B109" s="102" t="s">
+      <c r="A109" s="103"/>
+      <c r="B109" s="100" t="s">
         <v>245</v>
       </c>
       <c r="C109" s="7" t="s">
@@ -7041,8 +7041,8 @@
       <c r="N109" s="23"/>
     </row>
     <row r="110" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A110" s="105"/>
-      <c r="B110" s="102"/>
+      <c r="A110" s="103"/>
+      <c r="B110" s="100"/>
       <c r="C110" s="7" t="s">
         <v>172</v>
       </c>
@@ -7051,8 +7051,8 @@
       <c r="N110" s="25"/>
     </row>
     <row r="111" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A111" s="105"/>
-      <c r="B111" s="104" t="s">
+      <c r="A111" s="103"/>
+      <c r="B111" s="99" t="s">
         <v>173</v>
       </c>
       <c r="C111" s="6"/>
@@ -7063,8 +7063,8 @@
       <c r="N111" s="25"/>
     </row>
     <row r="112" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A112" s="105"/>
-      <c r="B112" s="104"/>
+      <c r="A112" s="103"/>
+      <c r="B112" s="99"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6" t="s">
         <v>215</v>
@@ -7075,8 +7075,8 @@
       <c r="N112" s="25"/>
     </row>
     <row r="113" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A113" s="105"/>
-      <c r="B113" s="104"/>
+      <c r="A113" s="103"/>
+      <c r="B113" s="99"/>
       <c r="C113" s="6" t="s">
         <v>173</v>
       </c>
@@ -7087,7 +7087,7 @@
       <c r="N113" s="26"/>
     </row>
     <row r="114" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A114" s="105"/>
+      <c r="A114" s="103"/>
       <c r="B114" s="13" t="s">
         <v>246</v>
       </c>
@@ -7103,7 +7103,7 @@
       <c r="N114" s="26"/>
     </row>
     <row r="115" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A115" s="105"/>
+      <c r="A115" s="103"/>
       <c r="B115" s="12" t="s">
         <v>174</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="N115" s="20"/>
     </row>
     <row r="116" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A116" s="105"/>
+      <c r="A116" s="103"/>
       <c r="B116" s="13" t="s">
         <v>247</v>
       </c>
@@ -7135,7 +7135,7 @@
       <c r="N116" s="21"/>
     </row>
     <row r="117" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A117" s="105"/>
+      <c r="A117" s="103"/>
       <c r="B117" s="12" t="s">
         <v>175</v>
       </c>
@@ -7151,7 +7151,7 @@
       <c r="N117" s="21"/>
     </row>
     <row r="118" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A118" s="105"/>
+      <c r="A118" s="103"/>
       <c r="B118" s="17" t="s">
         <v>248</v>
       </c>
@@ -7182,7 +7182,7 @@
       <c r="A121" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B121" s="104" t="s">
+      <c r="B121" s="99" t="s">
         <v>252</v>
       </c>
       <c r="C121" s="6"/>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="122" spans="1:14" ht="15.75" thickBot="1">
       <c r="A122" s="98"/>
-      <c r="B122" s="104"/>
+      <c r="B122" s="99"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6" t="s">
         <v>78</v>
@@ -7220,7 +7220,7 @@
     </row>
     <row r="124" spans="1:14" ht="15.75" thickBot="1">
       <c r="A124" s="98"/>
-      <c r="B124" s="102" t="s">
+      <c r="B124" s="100" t="s">
         <v>176</v>
       </c>
       <c r="C124" s="7"/>
@@ -7234,7 +7234,7 @@
     </row>
     <row r="125" spans="1:14" ht="15.75" thickBot="1">
       <c r="A125" s="98"/>
-      <c r="B125" s="102"/>
+      <c r="B125" s="100"/>
       <c r="C125" s="7" t="s">
         <v>176</v>
       </c>
@@ -7246,7 +7246,7 @@
     </row>
     <row r="126" spans="1:14" ht="15.75" thickBot="1">
       <c r="A126" s="98"/>
-      <c r="B126" s="104" t="s">
+      <c r="B126" s="99" t="s">
         <v>250</v>
       </c>
       <c r="C126" s="6" t="s">
@@ -7262,7 +7262,7 @@
     </row>
     <row r="127" spans="1:14" ht="15.75" thickBot="1">
       <c r="A127" s="98"/>
-      <c r="B127" s="104"/>
+      <c r="B127" s="99"/>
       <c r="C127" s="6"/>
       <c r="D127" s="6" t="s">
         <v>215</v>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="130" spans="1:14" ht="16.5" thickBot="1">
       <c r="A130" s="98"/>
-      <c r="B130" s="107" t="s">
+      <c r="B130" s="101" t="s">
         <v>182</v>
       </c>
       <c r="C130" s="7" t="s">
@@ -7322,7 +7322,7 @@
     </row>
     <row r="131" spans="1:14" ht="16.5" thickBot="1">
       <c r="A131" s="98"/>
-      <c r="B131" s="107"/>
+      <c r="B131" s="101"/>
       <c r="C131" s="7" t="s">
         <v>185</v>
       </c>
@@ -7336,7 +7336,7 @@
     </row>
     <row r="132" spans="1:14" ht="16.5" thickBot="1">
       <c r="A132" s="98"/>
-      <c r="B132" s="107"/>
+      <c r="B132" s="101"/>
       <c r="C132" s="7"/>
       <c r="D132" s="6" t="s">
         <v>215</v>
@@ -7380,7 +7380,7 @@
     </row>
     <row r="135" spans="1:14" ht="16.5" thickBot="1">
       <c r="A135" s="98"/>
-      <c r="B135" s="103" t="s">
+      <c r="B135" s="102" t="s">
         <v>254</v>
       </c>
       <c r="C135" s="6" t="s">
@@ -7396,7 +7396,7 @@
     </row>
     <row r="136" spans="1:14" ht="15.75" thickBot="1">
       <c r="A136" s="98"/>
-      <c r="B136" s="103"/>
+      <c r="B136" s="102"/>
       <c r="C136" s="6" t="s">
         <v>185</v>
       </c>
@@ -7410,7 +7410,7 @@
     </row>
     <row r="137" spans="1:14" ht="15.75" thickBot="1">
       <c r="A137" s="98"/>
-      <c r="B137" s="106" t="s">
+      <c r="B137" s="97" t="s">
         <v>785</v>
       </c>
       <c r="C137" s="17" t="s">
@@ -7426,7 +7426,7 @@
     </row>
     <row r="138" spans="1:14" ht="16.5" customHeight="1" thickBot="1">
       <c r="A138" s="98"/>
-      <c r="B138" s="106"/>
+      <c r="B138" s="97"/>
       <c r="E138" s="94" t="s">
         <v>783</v>
       </c>
@@ -7434,7 +7434,7 @@
     </row>
     <row r="139" spans="1:14" ht="16.5" customHeight="1" thickBot="1">
       <c r="A139" s="98"/>
-      <c r="B139" s="106"/>
+      <c r="B139" s="97"/>
       <c r="E139" s="94" t="s">
         <v>784</v>
       </c>
@@ -7571,13 +7571,16 @@
     </dataRefs>
   </dataConsolidate>
   <mergeCells count="32">
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="A121:A139"/>
-    <mergeCell ref="B121:B122"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="B130:B132"/>
-    <mergeCell ref="B135:B136"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="A2:A47"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
     <mergeCell ref="B87:B91"/>
     <mergeCell ref="B93:B95"/>
     <mergeCell ref="B96:B99"/>
@@ -7593,16 +7596,13 @@
     <mergeCell ref="B104:B108"/>
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="A2:A47"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="A121:A139"/>
+    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="B130:B132"/>
+    <mergeCell ref="B135:B136"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8793,8 +8793,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8835,10 +8835,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="100" t="s">
         <v>378</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="97" t="s">
         <v>560</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -8861,8 +8861,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A3" s="102"/>
-      <c r="B3" s="106"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="4" t="s">
         <v>389</v>
       </c>
@@ -8883,8 +8883,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A4" s="102"/>
-      <c r="B4" s="106"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="4" t="s">
         <v>390</v>
       </c>
@@ -8908,8 +8908,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A5" s="102"/>
-      <c r="B5" s="106"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="4" t="s">
         <v>391</v>
       </c>
@@ -8933,8 +8933,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A6" s="102"/>
-      <c r="B6" s="106"/>
+      <c r="A6" s="100"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="4" t="s">
         <v>392</v>
       </c>
@@ -8958,7 +8958,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A7" s="102"/>
+      <c r="A7" s="100"/>
       <c r="B7" s="67"/>
       <c r="C7" s="4" t="s">
         <v>215</v>
@@ -8980,7 +8980,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A8" s="102"/>
+      <c r="A8" s="100"/>
       <c r="B8" s="113" t="s">
         <v>561</v>
       </c>
@@ -9004,7 +9004,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A9" s="102"/>
+      <c r="A9" s="100"/>
       <c r="B9" s="113"/>
       <c r="C9" s="6" t="s">
         <v>395</v>
@@ -9023,7 +9023,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A10" s="102"/>
+      <c r="A10" s="100"/>
       <c r="B10" s="113"/>
       <c r="C10" s="6" t="s">
         <v>396</v>
@@ -9042,7 +9042,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A11" s="102"/>
+      <c r="A11" s="100"/>
       <c r="B11" s="68"/>
       <c r="C11" s="6" t="s">
         <v>215</v>
@@ -9061,8 +9061,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A12" s="102"/>
-      <c r="B12" s="106" t="s">
+      <c r="A12" s="100"/>
+      <c r="B12" s="97" t="s">
         <v>565</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -9082,8 +9082,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A13" s="102"/>
-      <c r="B13" s="106"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="7" t="s">
         <v>401</v>
       </c>
@@ -9101,8 +9101,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A14" s="102"/>
-      <c r="B14" s="106"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="7" t="s">
         <v>402</v>
       </c>
@@ -9120,8 +9120,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A15" s="102"/>
-      <c r="B15" s="106"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="7" t="s">
         <v>403</v>
       </c>
@@ -9139,8 +9139,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A16" s="102"/>
-      <c r="B16" s="106"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="7" t="s">
         <v>404</v>
       </c>
@@ -9156,8 +9156,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A17" s="102"/>
-      <c r="B17" s="106"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="7" t="s">
         <v>405</v>
       </c>
@@ -9173,7 +9173,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="102"/>
+      <c r="A18" s="100"/>
       <c r="B18" s="67"/>
       <c r="C18" s="7" t="s">
         <v>215</v>
@@ -9190,7 +9190,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A19" s="102"/>
+      <c r="A19" s="100"/>
       <c r="B19" s="114" t="s">
         <v>562</v>
       </c>
@@ -9211,7 +9211,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="102"/>
+      <c r="A20" s="100"/>
       <c r="B20" s="114"/>
       <c r="C20" s="6" t="s">
         <v>420</v>
@@ -9228,7 +9228,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A21" s="102"/>
+      <c r="A21" s="100"/>
       <c r="B21" s="114"/>
       <c r="C21" s="6" t="s">
         <v>421</v>
@@ -9245,7 +9245,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A22" s="102"/>
+      <c r="A22" s="100"/>
       <c r="B22" s="69"/>
       <c r="C22" s="6" t="s">
         <v>215</v>
@@ -9262,7 +9262,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A23" s="102"/>
+      <c r="A23" s="100"/>
       <c r="B23" s="110" t="s">
         <v>563</v>
       </c>
@@ -9283,7 +9283,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A24" s="102"/>
+      <c r="A24" s="100"/>
       <c r="B24" s="110"/>
       <c r="C24" s="4"/>
       <c r="D24" s="7" t="s">
@@ -9297,7 +9297,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="102"/>
+      <c r="A25" s="100"/>
       <c r="B25" s="110"/>
       <c r="C25" s="4"/>
       <c r="D25" s="7" t="s">
@@ -9311,7 +9311,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="102"/>
+      <c r="A26" s="100"/>
       <c r="B26" s="114" t="s">
         <v>381</v>
       </c>
@@ -9329,7 +9329,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A27" s="102"/>
+      <c r="A27" s="100"/>
       <c r="B27" s="114"/>
       <c r="C27" s="6" t="s">
         <v>426</v>
@@ -9343,7 +9343,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A28" s="102"/>
+      <c r="A28" s="100"/>
       <c r="B28" s="69"/>
       <c r="C28" s="6" t="s">
         <v>215</v>
@@ -9357,7 +9357,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A29" s="102"/>
+      <c r="A29" s="100"/>
       <c r="B29" s="40" t="s">
         <v>382</v>
       </c>
@@ -9375,7 +9375,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A30" s="102"/>
+      <c r="A30" s="100"/>
       <c r="B30" s="47" t="s">
         <v>558</v>
       </c>
@@ -9393,7 +9393,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A31" s="102"/>
+      <c r="A31" s="100"/>
       <c r="B31" s="40" t="s">
         <v>559</v>
       </c>
@@ -9411,7 +9411,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A32" s="102"/>
+      <c r="A32" s="100"/>
       <c r="B32" s="47" t="s">
         <v>383</v>
       </c>
@@ -9429,7 +9429,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A33" s="102"/>
+      <c r="A33" s="100"/>
       <c r="B33" s="40" t="s">
         <v>384</v>
       </c>
@@ -9447,7 +9447,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A34" s="102"/>
+      <c r="A34" s="100"/>
       <c r="B34" s="6" t="s">
         <v>385</v>
       </c>
@@ -9465,8 +9465,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="107" t="s">
+      <c r="A35" s="100"/>
+      <c r="B35" s="101" t="s">
         <v>564</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -9480,8 +9480,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A36" s="102"/>
-      <c r="B36" s="107"/>
+      <c r="A36" s="100"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="7" t="s">
         <v>413</v>
       </c>
@@ -9493,8 +9493,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A37" s="102"/>
-      <c r="B37" s="107"/>
+      <c r="A37" s="100"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="7" t="s">
         <v>414</v>
       </c>
@@ -9506,8 +9506,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A38" s="102"/>
-      <c r="B38" s="107"/>
+      <c r="A38" s="100"/>
+      <c r="B38" s="101"/>
       <c r="C38" s="7" t="s">
         <v>415</v>
       </c>
@@ -9519,7 +9519,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A39" s="102"/>
+      <c r="A39" s="100"/>
       <c r="B39" s="64"/>
       <c r="C39" s="7" t="s">
         <v>215</v>
@@ -9530,7 +9530,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A40" s="102"/>
+      <c r="A40" s="100"/>
       <c r="B40" s="6" t="s">
         <v>255</v>
       </c>
@@ -9663,7 +9663,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A51" s="104" t="s">
+      <c r="A51" s="99" t="s">
         <v>377</v>
       </c>
       <c r="B51" s="110" t="s">
@@ -9680,7 +9680,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A52" s="104"/>
+      <c r="A52" s="99"/>
       <c r="B52" s="110"/>
       <c r="C52" s="4"/>
       <c r="D52" s="7" t="s">
@@ -9691,7 +9691,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A53" s="104"/>
+      <c r="A53" s="99"/>
       <c r="B53" s="110"/>
       <c r="C53" s="4"/>
       <c r="D53" s="7" t="s">
@@ -49371,8 +49371,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AF298"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>